<commit_message>
PROS-5736 - CCRU - New Contract Execution KPIs
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Contract Execution 2018.xlsx
+++ b/Projects/CCRU/Data/Contract Execution 2018.xlsx
@@ -17,7 +17,8 @@
     <sheet name="Pos 2018 - Petroleum" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Pos 2018 - HoReCa - Bar Tavern Night Clubs" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Pos 2018 - HoReCa - Coffee Tea Shops" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Pos 2018 - FT" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Pos 2018 - HoReCa - Restaurant Cafe" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Pos 2018 - FT" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">'Pos 2018 - MT - Hypermarket'!$A$1:$AH$24</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="142">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -475,6 +476,12 @@
   <si>
     <t xml:space="preserve">HRC_CTS</t>
   </si>
+  <si>
+    <t xml:space="preserve">KPI Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HRC_RC</t>
+  </si>
 </sst>
 </file>
 
@@ -736,21 +743,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="4" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="4" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="22.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="67" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2220,20 +2227,1353 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="16.8542510121458"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" s="12" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AB2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" s="12" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF3" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0"/>
+      <c r="F4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="0"/>
+      <c r="I4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="2" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="0"/>
+      <c r="H5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0"/>
+      <c r="M5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="0"/>
+      <c r="H6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0"/>
+      <c r="M6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
+      <c r="T6" s="0"/>
+      <c r="U6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V6" s="0"/>
+      <c r="W6" s="0"/>
+      <c r="X6" s="0"/>
+      <c r="Y6" s="0"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="0"/>
+      <c r="AB6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="0"/>
+      <c r="H7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="0"/>
+      <c r="M7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0"/>
+      <c r="F8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="0"/>
+      <c r="I8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="2" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="0"/>
+      <c r="M9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="0"/>
+      <c r="M10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" s="0"/>
+      <c r="P10" s="0"/>
+      <c r="Q10" s="0"/>
+      <c r="R10" s="0"/>
+      <c r="S10" s="0"/>
+      <c r="T10" s="0"/>
+      <c r="U10" s="0"/>
+      <c r="V10" s="0"/>
+      <c r="W10" s="0"/>
+      <c r="X10" s="0"/>
+      <c r="Y10" s="0"/>
+      <c r="AA10" s="0"/>
+      <c r="AB10" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="D11" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="0"/>
+      <c r="M11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
+      <c r="Q11" s="0"/>
+      <c r="R11" s="0"/>
+      <c r="S11" s="0"/>
+      <c r="T11" s="0"/>
+      <c r="U11" s="0"/>
+      <c r="V11" s="0"/>
+      <c r="W11" s="0"/>
+      <c r="X11" s="0"/>
+      <c r="Y11" s="0"/>
+      <c r="AA11" s="0"/>
+      <c r="AB11" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="D12" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="0"/>
+      <c r="M12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="0"/>
+      <c r="P12" s="0"/>
+      <c r="Q12" s="0"/>
+      <c r="R12" s="0"/>
+      <c r="S12" s="0"/>
+      <c r="T12" s="0"/>
+      <c r="U12" s="0"/>
+      <c r="V12" s="0"/>
+      <c r="W12" s="0"/>
+      <c r="X12" s="0"/>
+      <c r="Y12" s="0"/>
+      <c r="AA12" s="0"/>
+      <c r="AB12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="0"/>
+      <c r="M13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O13" s="0"/>
+      <c r="P13" s="0"/>
+      <c r="Q13" s="0"/>
+      <c r="R13" s="0"/>
+      <c r="S13" s="0"/>
+      <c r="T13" s="0"/>
+      <c r="U13" s="0"/>
+      <c r="V13" s="0"/>
+      <c r="W13" s="0"/>
+      <c r="X13" s="0"/>
+      <c r="Y13" s="0"/>
+      <c r="AA13" s="0"/>
+      <c r="AB13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D14" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="0"/>
+      <c r="M14" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O14" s="0"/>
+      <c r="P14" s="0"/>
+      <c r="Q14" s="0"/>
+      <c r="R14" s="0"/>
+      <c r="S14" s="0"/>
+      <c r="T14" s="0"/>
+      <c r="U14" s="0"/>
+      <c r="V14" s="0"/>
+      <c r="W14" s="0"/>
+      <c r="X14" s="0"/>
+      <c r="Y14" s="0"/>
+      <c r="AA14" s="0"/>
+      <c r="AB14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="D15" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="0"/>
+      <c r="M15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" s="0"/>
+      <c r="P15" s="0"/>
+      <c r="Q15" s="0"/>
+      <c r="R15" s="0"/>
+      <c r="S15" s="0"/>
+      <c r="T15" s="0"/>
+      <c r="U15" s="0"/>
+      <c r="V15" s="0"/>
+      <c r="W15" s="0"/>
+      <c r="X15" s="0"/>
+      <c r="Y15" s="0"/>
+      <c r="AA15" s="0"/>
+      <c r="AB15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="D16" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="0"/>
+      <c r="M16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O16" s="0"/>
+      <c r="P16" s="0"/>
+      <c r="Q16" s="0"/>
+      <c r="R16" s="0"/>
+      <c r="S16" s="0"/>
+      <c r="T16" s="0"/>
+      <c r="U16" s="0"/>
+      <c r="V16" s="0"/>
+      <c r="W16" s="0"/>
+      <c r="X16" s="0"/>
+      <c r="Y16" s="0"/>
+      <c r="AA16" s="0"/>
+      <c r="AB16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D17" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="0"/>
+      <c r="M17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" s="0"/>
+      <c r="P17" s="0"/>
+      <c r="Q17" s="0"/>
+      <c r="R17" s="0"/>
+      <c r="S17" s="0"/>
+      <c r="T17" s="0"/>
+      <c r="U17" s="0"/>
+      <c r="V17" s="0"/>
+      <c r="W17" s="0"/>
+      <c r="X17" s="0"/>
+      <c r="Y17" s="0"/>
+      <c r="AA17" s="0"/>
+      <c r="AB17" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D18" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="0"/>
+      <c r="M18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" s="0"/>
+      <c r="P18" s="0"/>
+      <c r="Q18" s="0"/>
+      <c r="R18" s="0"/>
+      <c r="S18" s="0"/>
+      <c r="T18" s="0"/>
+      <c r="U18" s="0"/>
+      <c r="V18" s="0"/>
+      <c r="W18" s="0"/>
+      <c r="X18" s="0"/>
+      <c r="Y18" s="0"/>
+      <c r="AA18" s="0"/>
+      <c r="AB18" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="D19" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="0"/>
+      <c r="M19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O19" s="0"/>
+      <c r="P19" s="0"/>
+      <c r="Q19" s="0"/>
+      <c r="R19" s="0"/>
+      <c r="S19" s="0"/>
+      <c r="T19" s="0"/>
+      <c r="U19" s="0"/>
+      <c r="V19" s="0"/>
+      <c r="W19" s="0"/>
+      <c r="X19" s="0"/>
+      <c r="Y19" s="0"/>
+      <c r="AA19" s="0"/>
+      <c r="AB19" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="D20" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="K20" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="13"/>
+      <c r="M20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AF65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.1376518218624"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2378,21 +3718,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.995951417004"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="56" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3867,18 +5206,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="22.2793522267206"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="59" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5391,22 +6730,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="10.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="10.5708502024292"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.995951417004"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6879,20 +8218,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.8542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8217,20 +9556,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="22.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="22.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="23.5668016194332"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="80" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9555,21 +10894,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="2" width="12.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="20.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="2" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="21.2793522267206"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11075,22 +12414,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="25.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="26.995951417004"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12417,20 +13756,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.8542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="70" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-5736 - CCRU - New Contract Execution KPIs hot fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Contract Execution 2018.xlsx
+++ b/Projects/CCRU/Data/Contract Execution 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - MT - Hypermarket" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="141">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -355,9 +355,6 @@
   </si>
   <si>
     <t xml:space="preserve">Juices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PoS Set </t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
@@ -737,27 +734,27 @@
   </sheetPr>
   <dimension ref="A1:AK24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="4" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="4" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="23.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="67" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2221,26 +2218,26 @@
   </sheetPr>
   <dimension ref="A1:AF65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="16.8542510121458"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="16.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="17.5668016194332"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2248,7 +2245,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
@@ -2281,7 +2278,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>13</v>
@@ -2343,7 +2340,7 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -2393,7 +2390,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -2443,7 +2440,7 @@
     </row>
     <row r="4" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -2459,7 +2456,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
@@ -2501,7 +2498,7 @@
     </row>
     <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -2571,7 +2568,7 @@
     </row>
     <row r="6" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -2641,7 +2638,7 @@
     </row>
     <row r="7" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -2711,7 +2708,7 @@
     </row>
     <row r="8" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -2727,11 +2724,11 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>45</v>
@@ -2769,7 +2766,7 @@
     </row>
     <row r="9" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -2790,17 +2787,17 @@
         <v>5</v>
       </c>
       <c r="I9" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>111</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>49</v>
@@ -2833,7 +2830,7 @@
     </row>
     <row r="10" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -2854,17 +2851,17 @@
         <v>5</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>49</v>
@@ -2897,7 +2894,7 @@
     </row>
     <row r="11" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -2918,17 +2915,17 @@
         <v>5</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="0"/>
       <c r="M11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>49</v>
@@ -2961,7 +2958,7 @@
     </row>
     <row r="12" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -2982,17 +2979,17 @@
         <v>5</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="0"/>
       <c r="M12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>49</v>
@@ -3025,7 +3022,7 @@
     </row>
     <row r="13" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -3046,17 +3043,17 @@
         <v>5</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="0"/>
       <c r="M13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>49</v>
@@ -3089,7 +3086,7 @@
     </row>
     <row r="14" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -3110,17 +3107,17 @@
         <v>5</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="0"/>
       <c r="M14" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>49</v>
@@ -3153,7 +3150,7 @@
     </row>
     <row r="15" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -3174,17 +3171,17 @@
         <v>5</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>49</v>
@@ -3217,7 +3214,7 @@
     </row>
     <row r="16" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -3238,17 +3235,17 @@
         <v>5</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>49</v>
@@ -3281,7 +3278,7 @@
     </row>
     <row r="17" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -3302,17 +3299,17 @@
         <v>5</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>49</v>
@@ -3345,7 +3342,7 @@
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -3366,17 +3363,17 @@
         <v>5</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="0"/>
       <c r="M18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>49</v>
@@ -3409,7 +3406,7 @@
     </row>
     <row r="19" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -3430,17 +3427,17 @@
         <v>5</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>49</v>
@@ -3473,7 +3470,7 @@
     </row>
     <row r="20" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -3494,17 +3491,17 @@
         <v>5</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K20" s="14" t="n">
         <v>1</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>49</v>
@@ -3554,26 +3551,26 @@
   </sheetPr>
   <dimension ref="A1:AF65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="19.1376518218624"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.995951417004"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3614,7 +3611,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>13</v>
@@ -3712,26 +3709,27 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z2" activeCellId="0" sqref="Z2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="9"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.8542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="56" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3772,7 +3770,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>13</v>
@@ -3836,12 +3834,12 @@
       <c r="AI1" s="0"/>
       <c r="AJ1" s="0"/>
       <c r="AK1" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -3891,7 +3889,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -3941,7 +3939,7 @@
     </row>
     <row r="4" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -3999,7 +3997,7 @@
     </row>
     <row r="5" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -4060,7 +4058,7 @@
     </row>
     <row r="6" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -4121,7 +4119,7 @@
     </row>
     <row r="7" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -4182,7 +4180,7 @@
     </row>
     <row r="8" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -4243,7 +4241,7 @@
     </row>
     <row r="9" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -4304,7 +4302,7 @@
     </row>
     <row r="10" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -4365,7 +4363,7 @@
     </row>
     <row r="11" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -4426,7 +4424,7 @@
     </row>
     <row r="12" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -4487,7 +4485,7 @@
     </row>
     <row r="13" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -4548,7 +4546,7 @@
     </row>
     <row r="14" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -4609,7 +4607,7 @@
     </row>
     <row r="15" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -4657,7 +4655,7 @@
     </row>
     <row r="16" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -4717,7 +4715,7 @@
     </row>
     <row r="17" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -4777,7 +4775,7 @@
     </row>
     <row r="18" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -4836,7 +4834,7 @@
     </row>
     <row r="19" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -4883,7 +4881,7 @@
     </row>
     <row r="20" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -4943,7 +4941,7 @@
     </row>
     <row r="21" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>42</v>
@@ -5003,7 +5001,7 @@
     </row>
     <row r="22" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>42</v>
@@ -5063,7 +5061,7 @@
     </row>
     <row r="23" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>42</v>
@@ -5123,7 +5121,7 @@
     </row>
     <row r="24" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>42</v>
@@ -5200,24 +5198,24 @@
   </sheetPr>
   <dimension ref="A1:AJ65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE18" activeCellId="0" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="23.2793522267206"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="59" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5323,7 +5321,7 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -5373,7 +5371,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -5423,7 +5421,7 @@
     </row>
     <row r="4" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -5483,7 +5481,7 @@
     </row>
     <row r="5" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -5546,7 +5544,7 @@
     </row>
     <row r="6" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -5609,7 +5607,7 @@
     </row>
     <row r="7" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -5672,7 +5670,7 @@
     </row>
     <row r="8" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -5735,7 +5733,7 @@
     </row>
     <row r="9" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -5798,7 +5796,7 @@
     </row>
     <row r="10" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -5861,7 +5859,7 @@
     </row>
     <row r="11" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -5924,7 +5922,7 @@
     </row>
     <row r="12" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -5987,7 +5985,7 @@
     </row>
     <row r="13" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -6050,7 +6048,7 @@
     </row>
     <row r="14" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -6113,7 +6111,7 @@
     </row>
     <row r="15" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -6163,7 +6161,7 @@
     </row>
     <row r="16" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -6225,7 +6223,7 @@
     </row>
     <row r="17" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -6287,7 +6285,7 @@
     </row>
     <row r="18" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -6348,7 +6346,7 @@
     </row>
     <row r="19" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -6397,7 +6395,7 @@
     </row>
     <row r="20" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -6459,7 +6457,7 @@
     </row>
     <row r="21" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>42</v>
@@ -6521,7 +6519,7 @@
     </row>
     <row r="22" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>42</v>
@@ -6583,7 +6581,7 @@
     </row>
     <row r="23" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>42</v>
@@ -6645,7 +6643,7 @@
     </row>
     <row r="24" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>42</v>
@@ -6722,30 +6720,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK65536"/>
+  <dimension ref="1:24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z3" activeCellId="0" sqref="Z3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="10.5708502024292"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.8502024291498"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="10.995951417004"/>
+    <col collapsed="false" hidden="false" max="1023" min="38" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="21.8542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6850,10 +6849,11 @@
       <c r="AI1" s="0"/>
       <c r="AJ1" s="0"/>
       <c r="AK1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -6900,10 +6900,11 @@
       <c r="AF2" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -6950,10 +6951,11 @@
       <c r="AF3" s="13" t="s">
         <v>39</v>
       </c>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -7011,7 +7013,7 @@
     </row>
     <row r="5" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -7072,7 +7074,7 @@
     </row>
     <row r="6" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -7133,7 +7135,7 @@
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -7194,7 +7196,7 @@
     </row>
     <row r="8" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -7255,7 +7257,7 @@
     </row>
     <row r="9" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -7316,7 +7318,7 @@
     </row>
     <row r="10" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -7377,7 +7379,7 @@
     </row>
     <row r="11" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -7438,7 +7440,7 @@
     </row>
     <row r="12" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -7499,7 +7501,7 @@
     </row>
     <row r="13" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -7560,7 +7562,7 @@
     </row>
     <row r="14" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -7621,7 +7623,7 @@
     </row>
     <row r="15" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -7669,7 +7671,7 @@
     </row>
     <row r="16" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -7729,7 +7731,7 @@
     </row>
     <row r="17" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -7789,7 +7791,7 @@
     </row>
     <row r="18" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -7848,7 +7850,7 @@
     </row>
     <row r="19" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -7895,7 +7897,7 @@
     </row>
     <row r="20" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -7955,7 +7957,7 @@
     </row>
     <row r="21" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>42</v>
@@ -8015,7 +8017,7 @@
     </row>
     <row r="22" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>42</v>
@@ -8075,7 +8077,7 @@
     </row>
     <row r="23" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>42</v>
@@ -8135,7 +8137,7 @@
     </row>
     <row r="24" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>42</v>
@@ -8193,7 +8195,6 @@
         <v>39</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -8212,26 +8213,26 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="21.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8339,7 +8340,7 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -8389,7 +8390,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -8439,7 +8440,7 @@
     </row>
     <row r="4" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -8455,7 +8456,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
@@ -8484,7 +8485,7 @@
       </c>
       <c r="AA4" s="0"/>
       <c r="AB4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC4" s="19"/>
       <c r="AD4" s="19"/>
@@ -8497,7 +8498,7 @@
     </row>
     <row r="5" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -8567,7 +8568,7 @@
     </row>
     <row r="6" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -8637,7 +8638,7 @@
     </row>
     <row r="7" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -8707,7 +8708,7 @@
     </row>
     <row r="8" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -8723,11 +8724,11 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>45</v>
@@ -8752,7 +8753,7 @@
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC8" s="19"/>
       <c r="AD8" s="19"/>
@@ -8765,7 +8766,7 @@
     </row>
     <row r="9" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -8786,17 +8787,17 @@
         <v>5</v>
       </c>
       <c r="I9" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>111</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>49</v>
@@ -8829,7 +8830,7 @@
     </row>
     <row r="10" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -8850,17 +8851,17 @@
         <v>5</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>49</v>
@@ -8893,7 +8894,7 @@
     </row>
     <row r="11" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -8914,17 +8915,17 @@
         <v>5</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="0"/>
       <c r="M11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>49</v>
@@ -8957,7 +8958,7 @@
     </row>
     <row r="12" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -8978,17 +8979,17 @@
         <v>5</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="0"/>
       <c r="M12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>49</v>
@@ -9021,7 +9022,7 @@
     </row>
     <row r="13" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -9042,17 +9043,17 @@
         <v>5</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="0"/>
       <c r="M13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>49</v>
@@ -9085,7 +9086,7 @@
     </row>
     <row r="14" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -9106,17 +9107,17 @@
         <v>5</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="0"/>
       <c r="M14" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>49</v>
@@ -9149,7 +9150,7 @@
     </row>
     <row r="15" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -9170,17 +9171,17 @@
         <v>5</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>49</v>
@@ -9213,7 +9214,7 @@
     </row>
     <row r="16" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -9234,17 +9235,17 @@
         <v>5</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>49</v>
@@ -9277,7 +9278,7 @@
     </row>
     <row r="17" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -9298,17 +9299,17 @@
         <v>5</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>49</v>
@@ -9341,7 +9342,7 @@
     </row>
     <row r="18" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -9362,17 +9363,17 @@
         <v>5</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="0"/>
       <c r="M18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>49</v>
@@ -9405,7 +9406,7 @@
     </row>
     <row r="19" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -9426,17 +9427,17 @@
         <v>5</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>49</v>
@@ -9469,7 +9470,7 @@
     </row>
     <row r="20" customFormat="false" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -9490,17 +9491,17 @@
         <v>5</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K20" s="14" t="n">
         <v>1</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>49</v>
@@ -9550,26 +9551,26 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="24.5668016194332"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="80" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9677,7 +9678,7 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -9727,7 +9728,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -9777,7 +9778,7 @@
     </row>
     <row r="4" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -9793,7 +9794,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
@@ -9835,7 +9836,7 @@
     </row>
     <row r="5" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -9905,7 +9906,7 @@
     </row>
     <row r="6" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -9975,7 +9976,7 @@
     </row>
     <row r="7" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -10045,7 +10046,7 @@
     </row>
     <row r="8" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -10061,11 +10062,11 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>45</v>
@@ -10103,7 +10104,7 @@
     </row>
     <row r="9" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -10124,17 +10125,17 @@
         <v>5</v>
       </c>
       <c r="I9" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>111</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>49</v>
@@ -10167,7 +10168,7 @@
     </row>
     <row r="10" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -10188,17 +10189,17 @@
         <v>5</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>49</v>
@@ -10231,7 +10232,7 @@
     </row>
     <row r="11" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -10252,17 +10253,17 @@
         <v>5</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="0"/>
       <c r="M11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>49</v>
@@ -10295,7 +10296,7 @@
     </row>
     <row r="12" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -10316,17 +10317,17 @@
         <v>5</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="0"/>
       <c r="M12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>49</v>
@@ -10359,7 +10360,7 @@
     </row>
     <row r="13" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -10380,17 +10381,17 @@
         <v>5</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="0"/>
       <c r="M13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>49</v>
@@ -10423,7 +10424,7 @@
     </row>
     <row r="14" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -10444,17 +10445,17 @@
         <v>5</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="0"/>
       <c r="M14" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>49</v>
@@ -10487,7 +10488,7 @@
     </row>
     <row r="15" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -10508,17 +10509,17 @@
         <v>5</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>49</v>
@@ -10551,7 +10552,7 @@
     </row>
     <row r="16" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -10572,17 +10573,17 @@
         <v>5</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>49</v>
@@ -10615,7 +10616,7 @@
     </row>
     <row r="17" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -10636,17 +10637,17 @@
         <v>5</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>49</v>
@@ -10679,7 +10680,7 @@
     </row>
     <row r="18" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -10700,17 +10701,17 @@
         <v>5</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="0"/>
       <c r="M18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>49</v>
@@ -10743,7 +10744,7 @@
     </row>
     <row r="19" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -10764,17 +10765,17 @@
         <v>5</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>49</v>
@@ -10807,7 +10808,7 @@
     </row>
     <row r="20" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -10828,17 +10829,17 @@
         <v>5</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K20" s="14" t="n">
         <v>1</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>49</v>
@@ -10888,27 +10889,27 @@
   </sheetPr>
   <dimension ref="A1:AK26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="2" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="21.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.7125506072874"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="2" width="13.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="22.2793522267206"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11016,7 +11017,7 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -11066,7 +11067,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -11116,7 +11117,7 @@
     </row>
     <row r="4" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -11132,7 +11133,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
@@ -11164,7 +11165,7 @@
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -11224,7 +11225,7 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -11284,7 +11285,7 @@
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -11343,7 +11344,7 @@
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -11359,11 +11360,11 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>45</v>
@@ -11390,7 +11391,7 @@
     </row>
     <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -11412,17 +11413,17 @@
         <v>5</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>49</v>
@@ -11445,7 +11446,7 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -11467,17 +11468,17 @@
         <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>49</v>
@@ -11500,7 +11501,7 @@
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -11522,17 +11523,17 @@
         <v>5</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="0"/>
       <c r="M11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>49</v>
@@ -11555,7 +11556,7 @@
     </row>
     <row r="12" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -11577,17 +11578,17 @@
         <v>5</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="0"/>
       <c r="M12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>49</v>
@@ -11610,7 +11611,7 @@
     </row>
     <row r="13" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -11632,17 +11633,17 @@
         <v>5</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="0"/>
       <c r="M13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>49</v>
@@ -11665,7 +11666,7 @@
     </row>
     <row r="14" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -11687,17 +11688,17 @@
         <v>5</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="0"/>
       <c r="M14" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>49</v>
@@ -11720,7 +11721,7 @@
     </row>
     <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -11742,17 +11743,17 @@
         <v>5</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>49</v>
@@ -11775,7 +11776,7 @@
     </row>
     <row r="16" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -11797,17 +11798,17 @@
         <v>5</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>49</v>
@@ -11830,7 +11831,7 @@
     </row>
     <row r="17" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -11852,17 +11853,17 @@
         <v>5</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>49</v>
@@ -11885,7 +11886,7 @@
     </row>
     <row r="18" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -11907,17 +11908,17 @@
         <v>5</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="0"/>
       <c r="M18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>49</v>
@@ -11940,7 +11941,7 @@
     </row>
     <row r="19" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -11962,17 +11963,17 @@
         <v>5</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>49</v>
@@ -11995,7 +11996,7 @@
     </row>
     <row r="20" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -12017,17 +12018,17 @@
         <v>5</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K20" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L20" s="0"/>
       <c r="M20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>49</v>
@@ -12050,7 +12051,7 @@
     </row>
     <row r="21" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>42</v>
@@ -12066,7 +12067,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H21" s="0"/>
       <c r="I21" s="1" t="s">
@@ -12097,7 +12098,7 @@
     </row>
     <row r="22" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>42</v>
@@ -12156,7 +12157,7 @@
     </row>
     <row r="23" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>42</v>
@@ -12215,7 +12216,7 @@
     </row>
     <row r="24" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>42</v>
@@ -12274,7 +12275,7 @@
     </row>
     <row r="25" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>42</v>
@@ -12333,7 +12334,7 @@
     </row>
     <row r="26" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>42</v>
@@ -12408,28 +12409,28 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="28.1376518218623"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12537,7 +12538,7 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -12587,7 +12588,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -12637,7 +12638,7 @@
     </row>
     <row r="4" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -12653,7 +12654,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
@@ -12697,7 +12698,7 @@
     </row>
     <row r="5" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -12767,7 +12768,7 @@
     </row>
     <row r="6" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -12837,7 +12838,7 @@
     </row>
     <row r="7" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -12907,7 +12908,7 @@
     </row>
     <row r="8" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -12923,11 +12924,11 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>45</v>
@@ -12965,7 +12966,7 @@
     </row>
     <row r="9" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -12986,17 +12987,17 @@
         <v>5</v>
       </c>
       <c r="I9" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>111</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>49</v>
@@ -13029,7 +13030,7 @@
     </row>
     <row r="10" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -13050,17 +13051,17 @@
         <v>5</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>49</v>
@@ -13093,7 +13094,7 @@
     </row>
     <row r="11" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -13114,17 +13115,17 @@
         <v>5</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="0"/>
       <c r="M11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>49</v>
@@ -13157,7 +13158,7 @@
     </row>
     <row r="12" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -13178,17 +13179,17 @@
         <v>5</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="0"/>
       <c r="M12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>49</v>
@@ -13221,7 +13222,7 @@
     </row>
     <row r="13" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -13242,17 +13243,17 @@
         <v>5</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="0"/>
       <c r="M13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>49</v>
@@ -13285,7 +13286,7 @@
     </row>
     <row r="14" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -13306,17 +13307,17 @@
         <v>5</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="0"/>
       <c r="M14" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>49</v>
@@ -13349,7 +13350,7 @@
     </row>
     <row r="15" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -13370,17 +13371,17 @@
         <v>5</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>49</v>
@@ -13413,7 +13414,7 @@
     </row>
     <row r="16" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -13434,17 +13435,17 @@
         <v>5</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>49</v>
@@ -13477,7 +13478,7 @@
     </row>
     <row r="17" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -13498,17 +13499,17 @@
         <v>5</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>49</v>
@@ -13541,7 +13542,7 @@
     </row>
     <row r="18" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -13562,17 +13563,17 @@
         <v>5</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="0"/>
       <c r="M18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>49</v>
@@ -13605,7 +13606,7 @@
     </row>
     <row r="19" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -13626,17 +13627,17 @@
         <v>5</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>49</v>
@@ -13669,7 +13670,7 @@
     </row>
     <row r="20" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -13690,17 +13691,17 @@
         <v>5</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K20" s="14" t="n">
         <v>1</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>49</v>
@@ -13750,26 +13751,26 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="21.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="70" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13877,7 +13878,7 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -13927,7 +13928,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="38" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -13977,7 +13978,7 @@
     </row>
     <row r="4" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -13993,7 +13994,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
@@ -14035,7 +14036,7 @@
     </row>
     <row r="5" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -14105,7 +14106,7 @@
     </row>
     <row r="6" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -14175,7 +14176,7 @@
     </row>
     <row r="7" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -14245,7 +14246,7 @@
     </row>
     <row r="8" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -14261,11 +14262,11 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>45</v>
@@ -14303,7 +14304,7 @@
     </row>
     <row r="9" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -14324,17 +14325,17 @@
         <v>5</v>
       </c>
       <c r="I9" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>111</v>
       </c>
       <c r="K9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L9" s="0"/>
       <c r="M9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>49</v>
@@ -14367,7 +14368,7 @@
     </row>
     <row r="10" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -14388,17 +14389,17 @@
         <v>5</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>49</v>
@@ -14431,7 +14432,7 @@
     </row>
     <row r="11" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -14452,17 +14453,17 @@
         <v>5</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="0"/>
       <c r="M11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>49</v>
@@ -14495,7 +14496,7 @@
     </row>
     <row r="12" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -14516,17 +14517,17 @@
         <v>5</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L12" s="0"/>
       <c r="M12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>49</v>
@@ -14559,7 +14560,7 @@
     </row>
     <row r="13" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -14580,17 +14581,17 @@
         <v>5</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="0"/>
       <c r="M13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>49</v>
@@ -14623,7 +14624,7 @@
     </row>
     <row r="14" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -14644,17 +14645,17 @@
         <v>5</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L14" s="0"/>
       <c r="M14" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>49</v>
@@ -14687,7 +14688,7 @@
     </row>
     <row r="15" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -14708,17 +14709,17 @@
         <v>5</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L15" s="0"/>
       <c r="M15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>49</v>
@@ -14751,7 +14752,7 @@
     </row>
     <row r="16" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -14772,17 +14773,17 @@
         <v>5</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>49</v>
@@ -14815,7 +14816,7 @@
     </row>
     <row r="17" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -14836,17 +14837,17 @@
         <v>5</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L17" s="0"/>
       <c r="M17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>49</v>
@@ -14879,7 +14880,7 @@
     </row>
     <row r="18" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -14900,17 +14901,17 @@
         <v>5</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L18" s="0"/>
       <c r="M18" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>49</v>
@@ -14943,7 +14944,7 @@
     </row>
     <row r="19" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -14964,17 +14965,17 @@
         <v>5</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K19" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>49</v>
@@ -15007,7 +15008,7 @@
     </row>
     <row r="20" customFormat="false" ht="37" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -15028,17 +15029,17 @@
         <v>5</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K20" s="14" t="n">
         <v>1</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
CCRU template hot fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Contract Execution 2018.xlsx
+++ b/Projects/CCRU/Data/Contract Execution 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - MT - Hypermarket" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="140">
   <si>
     <t xml:space="preserve">Channel</t>
   </si>
@@ -474,9 +474,6 @@
     <t xml:space="preserve">HRC_CTS</t>
   </si>
   <si>
-    <t xml:space="preserve">KPI Set</t>
-  </si>
-  <si>
     <t xml:space="preserve">HRC_RC</t>
   </si>
 </sst>
@@ -734,27 +731,27 @@
   </sheetPr>
   <dimension ref="A1:AK24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="4" width="23.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="23.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="3" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="4" width="24.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="24.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="67" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2218,26 +2215,26 @@
   </sheetPr>
   <dimension ref="A1:AF65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.1376518218624"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="18.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="18.2834008097166"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2245,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>139</v>
+        <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
@@ -2340,7 +2337,7 @@
     </row>
     <row r="2" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>33</v>
@@ -2390,7 +2387,7 @@
     </row>
     <row r="3" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>33</v>
@@ -2440,7 +2437,7 @@
     </row>
     <row r="4" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>42</v>
@@ -2498,7 +2495,7 @@
     </row>
     <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>42</v>
@@ -2568,7 +2565,7 @@
     </row>
     <row r="6" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>42</v>
@@ -2638,7 +2635,7 @@
     </row>
     <row r="7" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>42</v>
@@ -2708,7 +2705,7 @@
     </row>
     <row r="8" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>42</v>
@@ -2766,7 +2763,7 @@
     </row>
     <row r="9" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>42</v>
@@ -2830,7 +2827,7 @@
     </row>
     <row r="10" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>42</v>
@@ -2894,7 +2891,7 @@
     </row>
     <row r="11" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>42</v>
@@ -2958,7 +2955,7 @@
     </row>
     <row r="12" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>42</v>
@@ -3022,7 +3019,7 @@
     </row>
     <row r="13" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>42</v>
@@ -3086,7 +3083,7 @@
     </row>
     <row r="14" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>42</v>
@@ -3150,7 +3147,7 @@
     </row>
     <row r="15" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>42</v>
@@ -3214,7 +3211,7 @@
     </row>
     <row r="16" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>42</v>
@@ -3278,7 +3275,7 @@
     </row>
     <row r="17" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>42</v>
@@ -3342,7 +3339,7 @@
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>42</v>
@@ -3406,7 +3403,7 @@
     </row>
     <row r="19" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>42</v>
@@ -3470,7 +3467,7 @@
     </row>
     <row r="20" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>42</v>
@@ -3551,26 +3548,26 @@
   </sheetPr>
   <dimension ref="A1:AF65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="19.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="19.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="25" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.8542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3709,27 +3706,27 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="9"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="20.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="9.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="21.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="56" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5198,24 +5195,24 @@
   </sheetPr>
   <dimension ref="A1:AJ65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AE18" activeCellId="0" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="24.2793522267206"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="59" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6722,29 +6719,29 @@
   </sheetPr>
   <dimension ref="1:24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="10.995951417004"/>
-    <col collapsed="false" hidden="false" max="1023" min="38" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="0" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1023" min="38" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="22.8502024291498"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8213,26 +8210,26 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q21" activeCellId="0" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="22.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9551,26 +9548,26 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="24.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="24.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="25.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="80" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10889,27 +10886,27 @@
   </sheetPr>
   <dimension ref="A1:AK26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.7125506072874"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="2" width="13.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.1417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="2" width="13.9959514170041"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.2793522267206"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="23.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="23.2793522267206"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12409,28 +12406,28 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="28.1376518218623"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="28.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="1" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="29.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="29.4210526315789"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13751,26 +13748,26 @@
   </sheetPr>
   <dimension ref="A1:AK65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="21.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="25" min="12" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="37" min="33" style="20" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="38" style="1" width="22.7085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="70" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>